<commit_message>
Fixed some bugs from the ctc office and added docstring comments to the line.
</commit_message>
<xml_diff>
--- a/system_data/schedules/schedule_1.xlsx
+++ b/system_data/schedules/schedule_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/system_data/schedules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28719A43-4486-4BDD-8780-5D8DB51467B9}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB343CAA-BB94-41F4-8037-C1939310A584}"/>
   <bookViews>
-    <workbookView xWindow="-37260" yWindow="1140" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -361,7 +361,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -390,7 +390,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>0.41666666666666669</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -401,7 +401,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1">
-        <v>0.42708333333333331</v>
+        <v>5.2083333333333336E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -412,7 +412,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>0.42708333333333331</v>
+        <v>5.2083333333333336E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -423,7 +423,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>0.4375</v>
+        <v>6.25E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed system_data folder overwrite.
</commit_message>
<xml_diff>
--- a/system_data/schedules/schedule_1.xlsx
+++ b/system_data/schedules/schedule_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/system_data/schedules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28719A43-4486-4BDD-8780-5D8DB51467B9}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB343CAA-BB94-41F4-8037-C1939310A584}"/>
   <bookViews>
-    <workbookView xWindow="-37260" yWindow="1140" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -361,7 +361,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -390,7 +390,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>0.41666666666666669</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -401,7 +401,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1">
-        <v>0.42708333333333331</v>
+        <v>5.2083333333333336E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -412,7 +412,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>0.42708333333333331</v>
+        <v>5.2083333333333336E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -423,7 +423,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>0.4375</v>
+        <v>6.25E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>